<commit_message>
fix soạn đơn, nhận hàng
</commit_message>
<xml_diff>
--- a/report/Test case/Test_Case_Truong.xlsx
+++ b/report/Test case/Test_Case_Truong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truon\Desktop\Chuyên đề di động\master\report\Test case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F00A71-94CC-4C15-BB6F-E8CA6A603B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8B77F4-0FD2-4415-A6E2-E175CFD4DF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="103">
   <si>
     <t>TC ID</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>LOW</t>
-  </si>
-  <si>
-    <t>NORMAL</t>
   </si>
   <si>
     <t>Check screen Display</t>
@@ -229,18 +226,152 @@
   </si>
   <si>
     <t>Screen "Thủ kho" -&gt;"Xem lại"</t>
+  </si>
+  <si>
+    <t>Listview</t>
+  </si>
+  <si>
+    <t>Thủ kho -&gt;"Xem lại"</t>
+  </si>
+  <si>
+    <t>Correctly display published books</t>
+  </si>
+  <si>
+    <t>the display is true to reality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No seleted combobox </t>
+  </si>
+  <si>
+    <t>1. Input username
+2.  input password
+3. No selected combobox and tab login</t>
+  </si>
+  <si>
+    <t>Message "You have not selected access rights "</t>
+  </si>
+  <si>
+    <t>add book and no selected combobox "Loại sách"</t>
+  </si>
+  <si>
+    <t>1. Input data full field 
+2. no selected combobox "Loại sách"
+3. Click "Thêm"</t>
+  </si>
+  <si>
+    <t>Message "You have not selected a book type"</t>
+  </si>
+  <si>
+    <t>No input field and tab button "Thêm"</t>
+  </si>
+  <si>
+    <t>1. No input data on field 
+2. Tab button "Thêm"</t>
+  </si>
+  <si>
+    <t>Message "You have not entered data "</t>
+  </si>
+  <si>
+    <t>don't enter the name field and click add</t>
+  </si>
+  <si>
+    <t>1. No input data on field name
+2. Tab button "Thêm"</t>
+  </si>
+  <si>
+    <t>Message "You have not entered name "</t>
+  </si>
+  <si>
+    <t>Long press on the item whose book is equal to 0</t>
+  </si>
+  <si>
+    <t>Long press on the item with a book other than 0</t>
+  </si>
+  <si>
+    <t>no remove item</t>
+  </si>
+  <si>
+    <t>Swipe up with your hand</t>
+  </si>
+  <si>
+    <t>Surf up</t>
+  </si>
+  <si>
+    <t>Download a new item</t>
+  </si>
+  <si>
+    <t>Drag the item to the left</t>
+  </si>
+  <si>
+    <t>Drag the item to the right</t>
+  </si>
+  <si>
+    <t>click on item</t>
+  </si>
+  <si>
+    <t>click button "Xem lại"</t>
+  </si>
+  <si>
+    <t>Go to the page to review the exported goods</t>
+  </si>
+  <si>
+    <t>No input "Số lượng"</t>
+  </si>
+  <si>
+    <t>1. seleted Lựa chọn loại sách
+2. selected Chọn tên
+3. No input "Số lượng"
+4. click Thêm</t>
+  </si>
+  <si>
+    <t>Message "You did not enter a number"</t>
+  </si>
+  <si>
+    <t>No input "Tên công ty nhập sách"</t>
+  </si>
+  <si>
+    <t>Message "You have not entered the company name"</t>
+  </si>
+  <si>
+    <t>Long click listview book</t>
+  </si>
+  <si>
+    <t>Check date</t>
+  </si>
+  <si>
+    <t>Show correct release date</t>
+  </si>
+  <si>
+    <t>Check quantity</t>
+  </si>
+  <si>
+    <t>Show the correct amount that was exported that day</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -307,7 +438,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -367,56 +498,121 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -694,17 +890,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.21875" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" customWidth="1"/>
     <col min="5" max="5" width="54.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -738,33 +934,33 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9"/>
+      <c r="A2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
@@ -780,19 +976,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
@@ -800,24 +996,24 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="43.2">
+    <row r="5" spans="1:9" ht="48" customHeight="1">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
+      <c r="B5" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
@@ -825,24 +1021,24 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="28.8">
+    <row r="6" spans="1:9" ht="43.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
@@ -850,24 +1046,24 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="28.8">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
@@ -880,19 +1076,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
@@ -901,61 +1097,61 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="28.8">
-      <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
@@ -963,24 +1159,24 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" ht="43.2">
       <c r="A12" s="2">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>2</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
@@ -988,24 +1184,24 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="43.2">
+    <row r="13" spans="1:9" ht="28.8">
       <c r="A13" s="2">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
@@ -1014,36 +1210,48 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="28.8">
       <c r="A15" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
@@ -1051,69 +1259,87 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" ht="28.8">
       <c r="A16" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>46</v>
+        <v>79</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+    <row r="17" spans="1:9" ht="43.2">
+      <c r="A17" s="2">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="12"/>
+      <c r="A18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2">
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
@@ -1125,46 +1351,70 @@
       <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="12"/>
+      <c r="A21" s="2">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
@@ -1174,22 +1424,22 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
@@ -1199,22 +1449,22 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
@@ -1223,61 +1473,61 @@
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="2">
-        <v>4</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="2"/>
+      <c r="A25" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="12"/>
+      <c r="A26" s="7">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="2">
-        <v>1</v>
+      <c r="A27" s="7">
+        <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>63</v>
+        <v>88</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
@@ -1286,23 +1536,23 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="2">
-        <v>2</v>
+      <c r="A28" s="7">
+        <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>63</v>
+        <v>89</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
@@ -1311,86 +1561,86 @@
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="2">
-        <v>3</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>59</v>
+      <c r="A29" s="7">
+        <v>4</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I29" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="2">
-        <v>4</v>
+      <c r="A30" s="7">
+        <v>5</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>63</v>
+        <v>90</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G30" s="2"/>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="2">
-        <v>5</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I31" s="2"/>
+      <c r="A31" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="2">
-        <v>6</v>
-      </c>
-      <c r="B32" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="C32" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="F32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
@@ -1399,54 +1649,415 @@
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="12"/>
+      <c r="A33" s="2">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="14">
-        <v>1</v>
+      <c r="A34" s="2">
+        <v>3</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="I34" s="2"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="14">
-        <v>2</v>
+      <c r="A35" s="2">
+        <v>4</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="14"/>
+      <c r="A36" s="2">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="2">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="10"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="2">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="2">
+        <v>2</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="2">
+        <v>3</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="2">
+        <v>4</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="2">
+        <v>5</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" ht="57.6">
+      <c r="A44" s="2">
+        <v>6</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="2">
+        <v>7</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="10"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="21">
+        <v>1</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="21">
+        <v>2</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="21">
+        <v>3</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I49" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A46:I46"/>
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A10:I10"/>
     <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A25:I25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix layout soan don
</commit_message>
<xml_diff>
--- a/report/Test case/Test_Case_Truong.xlsx
+++ b/report/Test case/Test_Case_Truong.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truon\Desktop\Chuyên đề di động\master\report\Test case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F00A71-94CC-4C15-BB6F-E8CA6A603B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8B77F4-0FD2-4415-A6E2-E175CFD4DF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="103">
   <si>
     <t>TC ID</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>LOW</t>
-  </si>
-  <si>
-    <t>NORMAL</t>
   </si>
   <si>
     <t>Check screen Display</t>
@@ -229,18 +226,152 @@
   </si>
   <si>
     <t>Screen "Thủ kho" -&gt;"Xem lại"</t>
+  </si>
+  <si>
+    <t>Listview</t>
+  </si>
+  <si>
+    <t>Thủ kho -&gt;"Xem lại"</t>
+  </si>
+  <si>
+    <t>Correctly display published books</t>
+  </si>
+  <si>
+    <t>the display is true to reality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No seleted combobox </t>
+  </si>
+  <si>
+    <t>1. Input username
+2.  input password
+3. No selected combobox and tab login</t>
+  </si>
+  <si>
+    <t>Message "You have not selected access rights "</t>
+  </si>
+  <si>
+    <t>add book and no selected combobox "Loại sách"</t>
+  </si>
+  <si>
+    <t>1. Input data full field 
+2. no selected combobox "Loại sách"
+3. Click "Thêm"</t>
+  </si>
+  <si>
+    <t>Message "You have not selected a book type"</t>
+  </si>
+  <si>
+    <t>No input field and tab button "Thêm"</t>
+  </si>
+  <si>
+    <t>1. No input data on field 
+2. Tab button "Thêm"</t>
+  </si>
+  <si>
+    <t>Message "You have not entered data "</t>
+  </si>
+  <si>
+    <t>don't enter the name field and click add</t>
+  </si>
+  <si>
+    <t>1. No input data on field name
+2. Tab button "Thêm"</t>
+  </si>
+  <si>
+    <t>Message "You have not entered name "</t>
+  </si>
+  <si>
+    <t>Long press on the item whose book is equal to 0</t>
+  </si>
+  <si>
+    <t>Long press on the item with a book other than 0</t>
+  </si>
+  <si>
+    <t>no remove item</t>
+  </si>
+  <si>
+    <t>Swipe up with your hand</t>
+  </si>
+  <si>
+    <t>Surf up</t>
+  </si>
+  <si>
+    <t>Download a new item</t>
+  </si>
+  <si>
+    <t>Drag the item to the left</t>
+  </si>
+  <si>
+    <t>Drag the item to the right</t>
+  </si>
+  <si>
+    <t>click on item</t>
+  </si>
+  <si>
+    <t>click button "Xem lại"</t>
+  </si>
+  <si>
+    <t>Go to the page to review the exported goods</t>
+  </si>
+  <si>
+    <t>No input "Số lượng"</t>
+  </si>
+  <si>
+    <t>1. seleted Lựa chọn loại sách
+2. selected Chọn tên
+3. No input "Số lượng"
+4. click Thêm</t>
+  </si>
+  <si>
+    <t>Message "You did not enter a number"</t>
+  </si>
+  <si>
+    <t>No input "Tên công ty nhập sách"</t>
+  </si>
+  <si>
+    <t>Message "You have not entered the company name"</t>
+  </si>
+  <si>
+    <t>Long click listview book</t>
+  </si>
+  <si>
+    <t>Check date</t>
+  </si>
+  <si>
+    <t>Show correct release date</t>
+  </si>
+  <si>
+    <t>Check quantity</t>
+  </si>
+  <si>
+    <t>Show the correct amount that was exported that day</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -307,7 +438,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -367,56 +498,121 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -694,17 +890,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.21875" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" customWidth="1"/>
     <col min="5" max="5" width="54.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -738,33 +934,33 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9"/>
+      <c r="A2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
@@ -780,19 +976,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
@@ -800,24 +996,24 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="43.2">
+    <row r="5" spans="1:9" ht="48" customHeight="1">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
+      <c r="B5" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
@@ -825,24 +1021,24 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="28.8">
+    <row r="6" spans="1:9" ht="43.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
@@ -850,24 +1046,24 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="28.8">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
@@ -880,19 +1076,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
@@ -901,61 +1097,61 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="28.8">
-      <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
@@ -963,24 +1159,24 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" ht="43.2">
       <c r="A12" s="2">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>2</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
@@ -988,24 +1184,24 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="43.2">
+    <row r="13" spans="1:9" ht="28.8">
       <c r="A13" s="2">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
@@ -1014,36 +1210,48 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" ht="28.8">
       <c r="A15" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
@@ -1051,69 +1259,87 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" ht="28.8">
       <c r="A16" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>46</v>
+        <v>79</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+    <row r="17" spans="1:9" ht="43.2">
+      <c r="A17" s="2">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="12"/>
+      <c r="A18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2">
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
@@ -1125,46 +1351,70 @@
       <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="12"/>
+      <c r="A21" s="2">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
@@ -1174,22 +1424,22 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2" t="s">
@@ -1199,22 +1449,22 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
@@ -1223,61 +1473,61 @@
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="2">
-        <v>4</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="2"/>
+      <c r="A25" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="12"/>
+      <c r="A26" s="7">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="2">
-        <v>1</v>
+      <c r="A27" s="7">
+        <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>63</v>
+        <v>88</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
@@ -1286,23 +1536,23 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="2">
-        <v>2</v>
+      <c r="A28" s="7">
+        <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>63</v>
+        <v>89</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
@@ -1311,86 +1561,86 @@
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="2">
-        <v>3</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>59</v>
+      <c r="A29" s="7">
+        <v>4</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I29" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="2">
-        <v>4</v>
+      <c r="A30" s="7">
+        <v>5</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>63</v>
+        <v>90</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G30" s="2"/>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="2">
-        <v>5</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I31" s="2"/>
+      <c r="A31" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="2">
-        <v>6</v>
-      </c>
-      <c r="B32" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="C32" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="F32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
@@ -1399,54 +1649,415 @@
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="12"/>
+      <c r="A33" s="2">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="14">
-        <v>1</v>
+      <c r="A34" s="2">
+        <v>3</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="I34" s="2"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="14">
-        <v>2</v>
+      <c r="A35" s="2">
+        <v>4</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="14"/>
+      <c r="A36" s="2">
+        <v>5</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="2">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="10"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="2">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="2">
+        <v>2</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="2">
+        <v>3</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="2">
+        <v>4</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="2">
+        <v>5</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" ht="57.6">
+      <c r="A44" s="2">
+        <v>6</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="2">
+        <v>7</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="10"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="21">
+        <v>1</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="21">
+        <v>2</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="21">
+        <v>3</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I49" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A46:I46"/>
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A10:I10"/>
     <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A25:I25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>